<commit_message>
Update MIF Tenplate schema
</commit_message>
<xml_diff>
--- a/template_examples/mIF_template.xlsx
+++ b/template_examples/mIF_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1575D4E3-1E2D-8E47-9B42-03E985EC4780}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2945E6-4638-6848-97AC-D7122B9E52DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="-18880" windowWidth="22920" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13020" yWindow="-18880" windowWidth="22920" windowHeight="13940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF_template" sheetId="1" r:id="rId1"/>
@@ -711,7 +711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2052,8 +2052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2069,7 +2069,9 @@
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1">
+        <v>10021</v>
+      </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>

</xml_diff>

<commit_message>
Final changes made to mif_template and micsss_template
</commit_message>
<xml_diff>
--- a/template_examples/mIF_template.xlsx
+++ b/template_examples/mIF_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38A286E-5E55-ED40-955A-D7A4A7DBFEBD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D64CB51-4C46-E34F-B34E-B3AB60842D89}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28440" windowHeight="16240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="27560" windowHeight="15700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF_template" sheetId="1" r:id="rId1"/>
@@ -88,25 +88,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Study related collection time point, as described in the protocol intake form. Example: Progression.</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="56">
   <si>
     <t>#t</t>
   </si>
@@ -126,6 +113,9 @@
     <t>STAINING PLATFORM</t>
   </si>
   <si>
+    <t>AUTOSTAINER MODEL</t>
+  </si>
+  <si>
     <t>IMAGE ANALYSIS SOFTWARE</t>
   </si>
   <si>
@@ -189,25 +179,28 @@
     <t>AMPLIFICATION TIME</t>
   </si>
   <si>
-    <t>CIMAC PARTICPANT ID</t>
-  </si>
-  <si>
-    <t>CIMAC SAMPLE ID</t>
-  </si>
-  <si>
-    <t>INTERNAL SLIDE ID</t>
-  </si>
-  <si>
-    <t>TIME POINT</t>
-  </si>
-  <si>
-    <t>STAINING DATE</t>
-  </si>
-  <si>
-    <t>IMAGING DATE</t>
-  </si>
-  <si>
-    <t>PROJECT INFORM FOLDER</t>
+    <t>CIMAC_PARTICPANT_ID</t>
+  </si>
+  <si>
+    <t>CIMAC_SAMPLE_ID</t>
+  </si>
+  <si>
+    <t>INTERNAL_SLIDE_ID</t>
+  </si>
+  <si>
+    <t>TIME_POINT</t>
+  </si>
+  <si>
+    <t>STAINING_DATE</t>
+  </si>
+  <si>
+    <t>IMAGING_DATE</t>
+  </si>
+  <si>
+    <t>IMAGING_STATUS</t>
+  </si>
+  <si>
+    <t>PROJECT_INFORM_FOLDER</t>
   </si>
   <si>
     <t>EXPORTED_DATA_FOLDER</t>
@@ -219,6 +212,9 @@
     <t>auto</t>
   </si>
   <si>
+    <t>Leica Bond RX</t>
+  </si>
+  <si>
     <t>InForm</t>
   </si>
   <si>
@@ -249,26 +245,29 @@
     <t>MA036-001</t>
   </si>
   <si>
-    <t>MA036-001 PRE</t>
-  </si>
-  <si>
-    <t>07FK 099</t>
+    <t>MA036-011 PRE</t>
+  </si>
+  <si>
+    <t>07FK099</t>
   </si>
   <si>
     <t>PRE</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>abc_inform</t>
+  </si>
+  <si>
     <t>ABC</t>
-  </si>
-  <si>
-    <t>ABC_INFIRM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,13 +288,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -362,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -373,17 +365,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N212"/>
+  <dimension ref="A1:N213"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -784,7 +767,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -806,7 +789,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -828,7 +811,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -842,7 +825,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -850,7 +833,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -864,7 +847,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -872,7 +855,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -894,7 +877,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -916,7 +899,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -930,1110 +913,1132 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
+      <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="5">
-        <v>3983272</v>
-      </c>
-      <c r="G13" s="4">
-        <v>2</v>
-      </c>
-      <c r="H13">
-        <v>520</v>
-      </c>
-      <c r="I13">
-        <v>2.8194444444444446</v>
-      </c>
-      <c r="J13" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" s="6">
-        <v>4.2361111111111106E-2</v>
-      </c>
-      <c r="L13" s="6">
-        <v>4.2361111111111106E-2</v>
-      </c>
-      <c r="M13" s="6">
-        <v>4.2361111111111106E-2</v>
-      </c>
-      <c r="N13" s="6">
-        <v>4.2361111111111106E-2</v>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14">
+        <v>39837272</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>520</v>
+      </c>
+      <c r="I14">
+        <v>3.5138888888888888</v>
+      </c>
+      <c r="J14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14">
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="L14" s="4">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="M14" s="4">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N14" s="4">
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:N1"/>
-    <mergeCell ref="B11:N11"/>
+    <mergeCell ref="B12:N12"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -2042,16 +2047,16 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"auto,manual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"InForm,QuPath"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"proprietary,watershed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"proprietary,random forest classifier"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L13:N212" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L14:N213" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
@@ -2065,7 +2070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -2099,7 +2104,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2108,1068 +2113,1080 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="8">
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="5">
         <v>35796</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="5">
         <v>35797</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" s="7"/>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B3:J3"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="F5:G204" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E204" xr:uid="{00000000-0002-0000-0100-000000000000}">
+      <formula1>"PRE,POST"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="F5:G204" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>AND(ISNUMBER(F5:F204),LEFT(CELL("format",F5:F204),1)="D")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H204" xr:uid="{00000000-0002-0000-0100-000003000000}">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mif datamodel dave (#30)
* mif_template validated

* Add miccss json schemas and template

* Changes made to micsss_template and mif_template

* Final changes made to mif_template and micsss_template
</commit_message>
<xml_diff>
--- a/template_examples/mIF_template.xlsx
+++ b/template_examples/mIF_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38A286E-5E55-ED40-955A-D7A4A7DBFEBD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8267FA-44DE-EB45-B217-F6740E978B3F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28440" windowHeight="16240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28280" windowHeight="16820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF_template" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="54">
   <si>
     <t>#t</t>
   </si>
@@ -126,6 +126,9 @@
     <t>STAINING PLATFORM</t>
   </si>
   <si>
+    <t>AUTOSTAINER MODEL</t>
+  </si>
+  <si>
     <t>IMAGE ANALYSIS SOFTWARE</t>
   </si>
   <si>
@@ -219,6 +222,9 @@
     <t>auto</t>
   </si>
   <si>
+    <t>Leica Bond RX</t>
+  </si>
+  <si>
     <t>InForm</t>
   </si>
   <si>
@@ -252,23 +258,23 @@
     <t>MA036-001 PRE</t>
   </si>
   <si>
-    <t>07FK 099</t>
+    <t>07FK099</t>
   </si>
   <si>
     <t>PRE</t>
   </si>
   <si>
+    <t>ABC_Inform</t>
+  </si>
+  <si>
     <t>ABC</t>
-  </si>
-  <si>
-    <t>ABC_INFIRM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,13 +295,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -362,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -373,17 +372,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N212"/>
+  <dimension ref="A1:N213"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -784,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -806,7 +796,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -828,7 +818,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -842,7 +832,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -850,7 +840,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -864,7 +854,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -872,7 +862,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -894,7 +884,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -916,7 +906,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -930,1110 +920,1132 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
+      <c r="C10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="5">
-        <v>3983272</v>
-      </c>
-      <c r="G13" s="4">
-        <v>2</v>
-      </c>
-      <c r="H13">
-        <v>520</v>
-      </c>
-      <c r="I13">
-        <v>2.8194444444444446</v>
-      </c>
-      <c r="J13" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" s="6">
-        <v>4.2361111111111106E-2</v>
-      </c>
-      <c r="L13" s="6">
-        <v>4.2361111111111106E-2</v>
-      </c>
-      <c r="M13" s="6">
-        <v>4.2361111111111106E-2</v>
-      </c>
-      <c r="N13" s="6">
-        <v>4.2361111111111106E-2</v>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14">
+        <v>3983272</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>520</v>
+      </c>
+      <c r="I14">
+        <v>3.5138888888888888</v>
+      </c>
+      <c r="J14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14">
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="L14" s="4">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="M14" s="4">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N14" s="4">
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:N1"/>
-    <mergeCell ref="B11:N11"/>
+    <mergeCell ref="B12:N12"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -2042,16 +2054,16 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"auto,manual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"InForm,QuPath"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"proprietary,watershed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"proprietary,random forest classifier"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L13:N212" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L14:N213" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
@@ -2065,8 +2077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2099,7 +2111,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2111,1056 +2123,1055 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="C5" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="8">
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="5">
         <v>35796</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="5">
         <v>35797</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" s="7"/>
+      <c r="H5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upload of new example_template
</commit_message>
<xml_diff>
--- a/template_examples/mIF_template.xlsx
+++ b/template_examples/mIF_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8267FA-44DE-EB45-B217-F6740E978B3F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3911653B-A237-B244-898C-9B2FB9C63BFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28280" windowHeight="16820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF_template" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="55">
   <si>
     <t>#t</t>
   </si>
@@ -210,6 +210,9 @@
     <t>IMAGING DATE</t>
   </si>
   <si>
+    <t>IMAGING STATUS</t>
+  </si>
+  <si>
     <t>PROJECT INFORM FOLDER</t>
   </si>
   <si>
@@ -222,31 +225,28 @@
     <t>auto</t>
   </si>
   <si>
-    <t>Leica Bond RX</t>
+    <t>fsadf</t>
   </si>
   <si>
     <t>InForm</t>
   </si>
   <si>
-    <t>2.4.2</t>
+    <t>fassdf</t>
   </si>
   <si>
     <t>proprietary</t>
   </si>
   <si>
-    <t>T-Cell HNSC</t>
-  </si>
-  <si>
-    <t>CD8</t>
-  </si>
-  <si>
-    <t>C8/144b</t>
-  </si>
-  <si>
-    <t>DAKO</t>
-  </si>
-  <si>
-    <t>C8-ABC</t>
+    <t>fasdfads</t>
+  </si>
+  <si>
+    <t>fdsfs</t>
+  </si>
+  <si>
+    <t>fdsfds</t>
+  </si>
+  <si>
+    <t>fsdaf</t>
   </si>
   <si>
     <t>DV</t>
@@ -255,7 +255,7 @@
     <t>MA036-001</t>
   </si>
   <si>
-    <t>MA036-001 PRE</t>
+    <t>MA036-001PRE</t>
   </si>
   <si>
     <t>07FK099</t>
@@ -264,7 +264,10 @@
     <t>PRE</t>
   </si>
   <si>
-    <t>ABC_Inform</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>ABC_Infform</t>
   </si>
   <si>
     <t>ABC</t>
@@ -774,7 +777,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -796,7 +799,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -818,7 +821,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -840,7 +843,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -862,7 +865,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -884,7 +887,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -906,7 +909,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -928,7 +931,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1008,28 +1011,28 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" t="s">
         <v>46</v>
       </c>
+      <c r="E14">
+        <v>10021</v>
+      </c>
       <c r="F14">
-        <v>3983272</v>
+        <v>20012</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>520</v>
       </c>
       <c r="I14">
-        <v>3.5138888888888888</v>
+        <v>2.8194444444444446</v>
       </c>
       <c r="J14" t="s">
         <v>47</v>
@@ -2077,8 +2080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2120,6 +2123,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2149,6 +2153,9 @@
       <c r="I4" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="J4" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -2170,7 +2177,7 @@
         <v>35796</v>
       </c>
       <c r="G5" s="5">
-        <v>35797</v>
+        <v>35796</v>
       </c>
       <c r="H5" t="s">
         <v>52</v>
@@ -2178,6 +2185,9 @@
       <c r="I5" t="s">
         <v>53</v>
       </c>
+      <c r="J5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3176,11 +3186,14 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B3:J3"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="F5:G204" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>AND(ISNUMBER(F5:F204),LEFT(CELL("format",F5:F204),1)="D")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H204" xr:uid="{00000000-0002-0000-0100-000002000000}">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Additional changes to file references
</commit_message>
<xml_diff>
--- a/template_examples/mIF_template.xlsx
+++ b/template_examples/mIF_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3911653B-A237-B244-898C-9B2FB9C63BFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9FB3CB-51B4-4B48-BD93-8C75A811298E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2800" yWindow="460" windowWidth="22060" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF_template" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="62">
   <si>
     <t>#t</t>
   </si>
@@ -120,6 +120,15 @@
     <t>LEAD ORGANIZATION STUDY ID</t>
   </si>
   <si>
+    <t>ASSAY CREATOR</t>
+  </si>
+  <si>
+    <t>EMAIL ADDRESS</t>
+  </si>
+  <si>
+    <t>UPLOADER</t>
+  </si>
+  <si>
     <t>SLIDE SCANNER MODEL</t>
   </si>
   <si>
@@ -219,34 +228,46 @@
     <t>EXPORTED_DATA_FOLDER</t>
   </si>
   <si>
+    <t>DFCI</t>
+  </si>
+  <si>
+    <t>jlo@jimmy.com</t>
+  </si>
+  <si>
+    <t>James Lindsay</t>
+  </si>
+  <si>
     <t>Vectra 2.0</t>
   </si>
   <si>
     <t>auto</t>
   </si>
   <si>
-    <t>fsadf</t>
+    <t>Leica Bond RX</t>
   </si>
   <si>
     <t>InForm</t>
   </si>
   <si>
-    <t>fassdf</t>
+    <t>2.4.2</t>
   </si>
   <si>
     <t>proprietary</t>
   </si>
   <si>
-    <t>fasdfads</t>
-  </si>
-  <si>
-    <t>fdsfs</t>
-  </si>
-  <si>
-    <t>fdsfds</t>
-  </si>
-  <si>
-    <t>fsdaf</t>
+    <t>T-Cell HNSC</t>
+  </si>
+  <si>
+    <t>CD8</t>
+  </si>
+  <si>
+    <t>C8/144b</t>
+  </si>
+  <si>
+    <t>DAKO</t>
+  </si>
+  <si>
+    <t>C8-ABC</t>
   </si>
   <si>
     <t>DV</t>
@@ -255,10 +276,10 @@
     <t>MA036-001</t>
   </si>
   <si>
-    <t>MA036-001PRE</t>
-  </si>
-  <si>
-    <t>07FK099</t>
+    <t>MA036-001 PRE</t>
+  </si>
+  <si>
+    <t>07FK 099</t>
   </si>
   <si>
     <t>PRE</t>
@@ -267,17 +288,17 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>ABC_Infform</t>
-  </si>
-  <si>
     <t>ABC</t>
+  </si>
+  <si>
+    <t>ABC_Inform</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +319,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -361,10 +390,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -375,10 +405,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -715,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N213"/>
+  <dimension ref="A1:N216"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -777,7 +811,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -798,8 +832,8 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>38</v>
+      <c r="C4" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -821,7 +855,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -843,7 +877,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -857,7 +891,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -865,7 +899,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -887,7 +921,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -909,7 +943,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -923,7 +957,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -931,7 +965,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -945,1134 +979,1203 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
+    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14">
-        <v>10021</v>
-      </c>
-      <c r="F14">
-        <v>20012</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>520</v>
-      </c>
-      <c r="I14">
-        <v>2.8194444444444446</v>
-      </c>
-      <c r="J14" t="s">
-        <v>47</v>
-      </c>
-      <c r="K14">
-        <v>0.11111111111111112</v>
-      </c>
-      <c r="L14" s="4">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="M14" s="4">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="N14" s="4">
-        <v>1.0416666666666666E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17">
+        <v>3983272</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>520</v>
+      </c>
+      <c r="I17">
+        <v>3.5138888888888888</v>
+      </c>
+      <c r="J17" t="s">
+        <v>54</v>
+      </c>
+      <c r="K17">
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="L17" s="5">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="M17" s="5">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N17" s="5">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:N1"/>
-    <mergeCell ref="B12:N12"/>
+    <mergeCell ref="B15:N15"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Vectra 2.0,Hamamatsu"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"auto,manual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"InForm,QuPath"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"proprietary,watershed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"proprietary,random forest classifier"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L14:N213" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L17:N216" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{9BF65C25-69BD-7840-8D38-33105368AF5C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2080,7 +2183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -2114,7 +2217,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2127,1061 +2230,1061 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="5">
+        <v>58</v>
+      </c>
+      <c r="F5" s="6">
         <v>35796</v>
       </c>
-      <c r="G5" s="5">
-        <v>35796</v>
+      <c r="G5" s="6">
+        <v>35797</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="I5" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4 json reference edits (#48)
* Edits to git repo folder org

* Edits made to json schema file names

* Created an assay core schema

* Edit references within json schemas

* Additional changes to file references

* re-applied changes after botched merge

* re-generated docs
</commit_message>
<xml_diff>
--- a/template_examples/mIF_template.xlsx
+++ b/template_examples/mIF_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3911653B-A237-B244-898C-9B2FB9C63BFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9FB3CB-51B4-4B48-BD93-8C75A811298E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2800" yWindow="460" windowWidth="22060" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF_template" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="62">
   <si>
     <t>#t</t>
   </si>
@@ -120,6 +120,15 @@
     <t>LEAD ORGANIZATION STUDY ID</t>
   </si>
   <si>
+    <t>ASSAY CREATOR</t>
+  </si>
+  <si>
+    <t>EMAIL ADDRESS</t>
+  </si>
+  <si>
+    <t>UPLOADER</t>
+  </si>
+  <si>
     <t>SLIDE SCANNER MODEL</t>
   </si>
   <si>
@@ -219,34 +228,46 @@
     <t>EXPORTED_DATA_FOLDER</t>
   </si>
   <si>
+    <t>DFCI</t>
+  </si>
+  <si>
+    <t>jlo@jimmy.com</t>
+  </si>
+  <si>
+    <t>James Lindsay</t>
+  </si>
+  <si>
     <t>Vectra 2.0</t>
   </si>
   <si>
     <t>auto</t>
   </si>
   <si>
-    <t>fsadf</t>
+    <t>Leica Bond RX</t>
   </si>
   <si>
     <t>InForm</t>
   </si>
   <si>
-    <t>fassdf</t>
+    <t>2.4.2</t>
   </si>
   <si>
     <t>proprietary</t>
   </si>
   <si>
-    <t>fasdfads</t>
-  </si>
-  <si>
-    <t>fdsfs</t>
-  </si>
-  <si>
-    <t>fdsfds</t>
-  </si>
-  <si>
-    <t>fsdaf</t>
+    <t>T-Cell HNSC</t>
+  </si>
+  <si>
+    <t>CD8</t>
+  </si>
+  <si>
+    <t>C8/144b</t>
+  </si>
+  <si>
+    <t>DAKO</t>
+  </si>
+  <si>
+    <t>C8-ABC</t>
   </si>
   <si>
     <t>DV</t>
@@ -255,10 +276,10 @@
     <t>MA036-001</t>
   </si>
   <si>
-    <t>MA036-001PRE</t>
-  </si>
-  <si>
-    <t>07FK099</t>
+    <t>MA036-001 PRE</t>
+  </si>
+  <si>
+    <t>07FK 099</t>
   </si>
   <si>
     <t>PRE</t>
@@ -267,17 +288,17 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>ABC_Infform</t>
-  </si>
-  <si>
     <t>ABC</t>
+  </si>
+  <si>
+    <t>ABC_Inform</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +319,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -361,10 +390,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -375,10 +405,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -715,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N213"/>
+  <dimension ref="A1:N216"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -777,7 +811,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -798,8 +832,8 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>38</v>
+      <c r="C4" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -821,7 +855,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -843,7 +877,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -857,7 +891,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -865,7 +899,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -887,7 +921,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -909,7 +943,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -923,7 +957,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -931,7 +965,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -945,1134 +979,1203 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
+    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14">
-        <v>10021</v>
-      </c>
-      <c r="F14">
-        <v>20012</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>520</v>
-      </c>
-      <c r="I14">
-        <v>2.8194444444444446</v>
-      </c>
-      <c r="J14" t="s">
-        <v>47</v>
-      </c>
-      <c r="K14">
-        <v>0.11111111111111112</v>
-      </c>
-      <c r="L14" s="4">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="M14" s="4">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="N14" s="4">
-        <v>1.0416666666666666E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17">
+        <v>3983272</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>520</v>
+      </c>
+      <c r="I17">
+        <v>3.5138888888888888</v>
+      </c>
+      <c r="J17" t="s">
+        <v>54</v>
+      </c>
+      <c r="K17">
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="L17" s="5">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="M17" s="5">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N17" s="5">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:N1"/>
-    <mergeCell ref="B12:N12"/>
+    <mergeCell ref="B15:N15"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Vectra 2.0,Hamamatsu"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"auto,manual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"InForm,QuPath"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"proprietary,watershed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"proprietary,random forest classifier"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L14:N213" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L17:N216" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{9BF65C25-69BD-7840-8D38-33105368AF5C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2080,7 +2183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -2114,7 +2217,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2127,1061 +2230,1061 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="5">
+        <v>58</v>
+      </c>
+      <c r="F5" s="6">
         <v>35796</v>
       </c>
-      <c r="G5" s="5">
-        <v>35796</v>
+      <c r="G5" s="6">
+        <v>35797</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="I5" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additional changes to assay core, and corresponding templates
</commit_message>
<xml_diff>
--- a/template_examples/mIF_template.xlsx
+++ b/template_examples/mIF_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9FB3CB-51B4-4B48-BD93-8C75A811298E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFA8E12-3166-7343-B4C4-AFD35169C723}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="460" windowWidth="22060" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4180" yWindow="-20100" windowWidth="22200" windowHeight="16560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF_template" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,32 @@
             <family val="2"/>
           </rPr>
           <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates what site is filling out the assay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assay category.</t>
         </r>
       </text>
     </comment>
@@ -106,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="91">
   <si>
     <t>#t</t>
   </si>
@@ -123,10 +149,7 @@
     <t>ASSAY CREATOR</t>
   </si>
   <si>
-    <t>EMAIL ADDRESS</t>
-  </si>
-  <si>
-    <t>UPLOADER</t>
+    <t>ASSAY CATEGORY</t>
   </si>
   <si>
     <t>SLIDE SCANNER MODEL</t>
@@ -231,10 +254,7 @@
     <t>DFCI</t>
   </si>
   <si>
-    <t>jlo@jimmy.com</t>
-  </si>
-  <si>
-    <t>James Lindsay</t>
+    <t>Multiplex Immunofluorescence</t>
   </si>
   <si>
     <t>Vectra 2.0</t>
@@ -243,21 +263,60 @@
     <t>auto</t>
   </si>
   <si>
-    <t>Leica Bond RX</t>
+    <t>Leica Model</t>
   </si>
   <si>
     <t>InForm</t>
   </si>
   <si>
-    <t>2.4.2</t>
-  </si>
-  <si>
     <t>proprietary</t>
   </si>
   <si>
     <t>T-Cell HNSC</t>
   </si>
   <si>
+    <t>MA036-001</t>
+  </si>
+  <si>
+    <t>MA036-001 PRE</t>
+  </si>
+  <si>
+    <t>07FK 099</t>
+  </si>
+  <si>
+    <t>PRE</t>
+  </si>
+  <si>
+    <t>ABC_INFORM</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>MA036-002</t>
+  </si>
+  <si>
+    <t>BS-18-38992 A2</t>
+  </si>
+  <si>
+    <t>4KHI 021</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>MA036-003</t>
+  </si>
+  <si>
+    <t>MA036-003 C1D1</t>
+  </si>
+  <si>
+    <t>8KBI 022</t>
+  </si>
+  <si>
+    <t>C1D1</t>
+  </si>
+  <si>
     <t>CD8</t>
   </si>
   <si>
@@ -273,25 +332,79 @@
     <t>DV</t>
   </si>
   <si>
-    <t>MA036-001</t>
-  </si>
-  <si>
-    <t>MA036-001 PRE</t>
-  </si>
-  <si>
-    <t>07FK 099</t>
-  </si>
-  <si>
-    <t>PRE</t>
+    <t>1:100</t>
+  </si>
+  <si>
+    <t>PD-L1</t>
+  </si>
+  <si>
+    <t>9A11</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>9A-ABC</t>
+  </si>
+  <si>
+    <t>1:500</t>
+  </si>
+  <si>
+    <t>VENTANA</t>
+  </si>
+  <si>
+    <t>1:200</t>
+  </si>
+  <si>
+    <t>CD3</t>
+  </si>
+  <si>
+    <t>A0452</t>
+  </si>
+  <si>
+    <t>A0-ABC</t>
+  </si>
+  <si>
+    <t>PD-1</t>
+  </si>
+  <si>
+    <t>EH33</t>
+  </si>
+  <si>
+    <t>EH-ABC</t>
+  </si>
+  <si>
+    <t>1:150</t>
+  </si>
+  <si>
+    <t>Cytokeratin</t>
+  </si>
+  <si>
+    <t>A1/A3</t>
+  </si>
+  <si>
+    <t>A1-ABC</t>
+  </si>
+  <si>
+    <t>1:2000</t>
+  </si>
+  <si>
+    <t>1:50</t>
+  </si>
+  <si>
+    <t>1:5000</t>
+  </si>
+  <si>
+    <t>1:1000</t>
+  </si>
+  <si>
+    <t>1:11000</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>ABC_Inform</t>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -321,9 +434,8 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -390,11 +502,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -402,17 +513,37 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -749,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N216"/>
+  <dimension ref="A1:N215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -765,21 +896,21 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -811,7 +942,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -832,8 +963,8 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>41</v>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -855,7 +986,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -877,7 +1008,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -899,7 +1030,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -921,7 +1052,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -935,7 +1066,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -943,7 +1074,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -957,7 +1088,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -965,7 +1096,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -987,7 +1118,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1009,7 +1140,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1023,1159 +1154,1296 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="5">
+        <v>3983272</v>
+      </c>
+      <c r="G16" s="4">
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H16" s="4">
+        <v>520</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16" s="11">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="M16" s="11">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N16" s="11">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17">
-        <v>3983272</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-      <c r="H17">
-        <v>520</v>
-      </c>
-      <c r="I17">
-        <v>3.5138888888888888</v>
-      </c>
-      <c r="J17" t="s">
-        <v>54</v>
-      </c>
-      <c r="K17">
-        <v>0.11111111111111112</v>
-      </c>
-      <c r="L17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="5">
+        <v>29387234</v>
+      </c>
+      <c r="G17" s="4">
+        <v>3</v>
+      </c>
+      <c r="H17" s="4">
+        <v>540</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L17" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="M17" s="11">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N17" s="11">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="5">
+        <v>2881947</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4">
+        <v>570</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L18" s="12">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M18" s="11">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N17" s="5">
+      <c r="N18" s="11">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="5">
+        <v>293872</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4</v>
+      </c>
+      <c r="H19" s="4">
+        <v>620</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="M19" s="11">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N19" s="11">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="5">
+        <v>392835</v>
+      </c>
+      <c r="G20" s="4">
+        <v>5</v>
+      </c>
+      <c r="H20" s="4">
+        <v>690</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="L20" s="11">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="M20" s="11">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N20" s="11">
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A216" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:N1"/>
-    <mergeCell ref="B15:N15"/>
+    <mergeCell ref="B14:N14"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Vectra 2.0,Hamamatsu"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"auto,manual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"InForm,QuPath"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"proprietary,watershed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"proprietary,random forest classifier"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L17:N216" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L16:N17 M18:N18 L19:N215" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{9BF65C25-69BD-7840-8D38-33105368AF5C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2183,8 +2451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2216,1075 +2484,1129 @@
       <c r="N1" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="B3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="6">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="10">
         <v>35796</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="10">
         <v>35797</v>
       </c>
-      <c r="H5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J5" t="s">
-        <v>60</v>
+      <c r="H5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="10">
+        <v>35797</v>
+      </c>
+      <c r="G6" s="10">
+        <v>35797</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="10">
+        <v>35798</v>
+      </c>
+      <c r="G7" s="10">
+        <v>35797</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change assay core (#51)
* Removed Email Address property from templates

* Additional changes to assay core, and corresponding templates

* updated docs to reflect changes
</commit_message>
<xml_diff>
--- a/template_examples/mIF_template.xlsx
+++ b/template_examples/mIF_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9FB3CB-51B4-4B48-BD93-8C75A811298E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFA8E12-3166-7343-B4C4-AFD35169C723}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="460" windowWidth="22060" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4180" yWindow="-20100" windowWidth="22200" windowHeight="16560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF_template" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,32 @@
             <family val="2"/>
           </rPr>
           <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates what site is filling out the assay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assay category.</t>
         </r>
       </text>
     </comment>
@@ -106,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="91">
   <si>
     <t>#t</t>
   </si>
@@ -123,10 +149,7 @@
     <t>ASSAY CREATOR</t>
   </si>
   <si>
-    <t>EMAIL ADDRESS</t>
-  </si>
-  <si>
-    <t>UPLOADER</t>
+    <t>ASSAY CATEGORY</t>
   </si>
   <si>
     <t>SLIDE SCANNER MODEL</t>
@@ -231,10 +254,7 @@
     <t>DFCI</t>
   </si>
   <si>
-    <t>jlo@jimmy.com</t>
-  </si>
-  <si>
-    <t>James Lindsay</t>
+    <t>Multiplex Immunofluorescence</t>
   </si>
   <si>
     <t>Vectra 2.0</t>
@@ -243,21 +263,60 @@
     <t>auto</t>
   </si>
   <si>
-    <t>Leica Bond RX</t>
+    <t>Leica Model</t>
   </si>
   <si>
     <t>InForm</t>
   </si>
   <si>
-    <t>2.4.2</t>
-  </si>
-  <si>
     <t>proprietary</t>
   </si>
   <si>
     <t>T-Cell HNSC</t>
   </si>
   <si>
+    <t>MA036-001</t>
+  </si>
+  <si>
+    <t>MA036-001 PRE</t>
+  </si>
+  <si>
+    <t>07FK 099</t>
+  </si>
+  <si>
+    <t>PRE</t>
+  </si>
+  <si>
+    <t>ABC_INFORM</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>MA036-002</t>
+  </si>
+  <si>
+    <t>BS-18-38992 A2</t>
+  </si>
+  <si>
+    <t>4KHI 021</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>MA036-003</t>
+  </si>
+  <si>
+    <t>MA036-003 C1D1</t>
+  </si>
+  <si>
+    <t>8KBI 022</t>
+  </si>
+  <si>
+    <t>C1D1</t>
+  </si>
+  <si>
     <t>CD8</t>
   </si>
   <si>
@@ -273,25 +332,79 @@
     <t>DV</t>
   </si>
   <si>
-    <t>MA036-001</t>
-  </si>
-  <si>
-    <t>MA036-001 PRE</t>
-  </si>
-  <si>
-    <t>07FK 099</t>
-  </si>
-  <si>
-    <t>PRE</t>
+    <t>1:100</t>
+  </si>
+  <si>
+    <t>PD-L1</t>
+  </si>
+  <si>
+    <t>9A11</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>9A-ABC</t>
+  </si>
+  <si>
+    <t>1:500</t>
+  </si>
+  <si>
+    <t>VENTANA</t>
+  </si>
+  <si>
+    <t>1:200</t>
+  </si>
+  <si>
+    <t>CD3</t>
+  </si>
+  <si>
+    <t>A0452</t>
+  </si>
+  <si>
+    <t>A0-ABC</t>
+  </si>
+  <si>
+    <t>PD-1</t>
+  </si>
+  <si>
+    <t>EH33</t>
+  </si>
+  <si>
+    <t>EH-ABC</t>
+  </si>
+  <si>
+    <t>1:150</t>
+  </si>
+  <si>
+    <t>Cytokeratin</t>
+  </si>
+  <si>
+    <t>A1/A3</t>
+  </si>
+  <si>
+    <t>A1-ABC</t>
+  </si>
+  <si>
+    <t>1:2000</t>
+  </si>
+  <si>
+    <t>1:50</t>
+  </si>
+  <si>
+    <t>1:5000</t>
+  </si>
+  <si>
+    <t>1:1000</t>
+  </si>
+  <si>
+    <t>1:11000</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>ABC_Inform</t>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -321,9 +434,8 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -390,11 +502,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -402,17 +513,37 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -749,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N216"/>
+  <dimension ref="A1:N215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -765,21 +896,21 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -811,7 +942,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -832,8 +963,8 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>41</v>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -855,7 +986,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -877,7 +1008,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -899,7 +1030,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -921,7 +1052,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -935,7 +1066,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -943,7 +1074,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -957,7 +1088,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -965,7 +1096,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -987,7 +1118,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1009,7 +1140,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1023,1159 +1154,1296 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="5">
+        <v>3983272</v>
+      </c>
+      <c r="G16" s="4">
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H16" s="4">
+        <v>520</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16" s="11">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="M16" s="11">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N16" s="11">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17">
-        <v>3983272</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-      <c r="H17">
-        <v>520</v>
-      </c>
-      <c r="I17">
-        <v>3.5138888888888888</v>
-      </c>
-      <c r="J17" t="s">
-        <v>54</v>
-      </c>
-      <c r="K17">
-        <v>0.11111111111111112</v>
-      </c>
-      <c r="L17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="5">
+        <v>29387234</v>
+      </c>
+      <c r="G17" s="4">
+        <v>3</v>
+      </c>
+      <c r="H17" s="4">
+        <v>540</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L17" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="M17" s="11">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N17" s="11">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="5">
+        <v>2881947</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4">
+        <v>570</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L18" s="12">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M18" s="11">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N17" s="5">
+      <c r="N18" s="11">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="5">
+        <v>293872</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4</v>
+      </c>
+      <c r="H19" s="4">
+        <v>620</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="M19" s="11">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N19" s="11">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="5">
+        <v>392835</v>
+      </c>
+      <c r="G20" s="4">
+        <v>5</v>
+      </c>
+      <c r="H20" s="4">
+        <v>690</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="L20" s="11">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="M20" s="11">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N20" s="11">
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A216" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:N1"/>
-    <mergeCell ref="B15:N15"/>
+    <mergeCell ref="B14:N14"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Vectra 2.0,Hamamatsu"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"auto,manual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"InForm,QuPath"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"proprietary,watershed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"proprietary,random forest classifier"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L17:N216" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L16:N17 M18:N18 L19:N215" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{9BF65C25-69BD-7840-8D38-33105368AF5C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2183,8 +2451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2216,1075 +2484,1129 @@
       <c r="N1" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="B3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="6">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="10">
         <v>35796</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="10">
         <v>35797</v>
       </c>
-      <c r="H5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J5" t="s">
-        <v>60</v>
+      <c r="H5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="10">
+        <v>35797</v>
+      </c>
+      <c r="G6" s="10">
+        <v>35797</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="10">
+        <v>35798</v>
+      </c>
+      <c r="G7" s="10">
+        <v>35797</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Regenerated and validated json templates
</commit_message>
<xml_diff>
--- a/template_examples/mIF_template.xlsx
+++ b/template_examples/mIF_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFA8E12-3166-7343-B4C4-AFD35169C723}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478EAFFD-1742-B94D-BB85-373DD1D8B4C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4180" yWindow="-20100" windowWidth="22200" windowHeight="16560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-860" yWindow="-19460" windowWidth="22680" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF_template" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="92">
   <si>
     <t>#t</t>
   </si>
@@ -236,6 +236,9 @@
     <t>TIME POINT</t>
   </si>
   <si>
+    <t>PROTOCOL_NAME</t>
+  </si>
+  <si>
     <t>STAINING DATE</t>
   </si>
   <si>
@@ -263,18 +266,105 @@
     <t>auto</t>
   </si>
   <si>
-    <t>Leica Model</t>
+    <t>Leica Bon RX</t>
   </si>
   <si>
     <t>InForm</t>
   </si>
   <si>
+    <t>2.4.2</t>
+  </si>
+  <si>
     <t>proprietary</t>
   </si>
   <si>
     <t>T-Cell HNSC</t>
   </si>
   <si>
+    <t>CD8</t>
+  </si>
+  <si>
+    <t>C8/144b</t>
+  </si>
+  <si>
+    <t>DAKO</t>
+  </si>
+  <si>
+    <t>C8-ABC</t>
+  </si>
+  <si>
+    <t>1:5,000</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>1:100</t>
+  </si>
+  <si>
+    <t>PD-L1</t>
+  </si>
+  <si>
+    <t>9A11</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>9A-ABC</t>
+  </si>
+  <si>
+    <t>1:500</t>
+  </si>
+  <si>
+    <t>VENTANA</t>
+  </si>
+  <si>
+    <t>1:200</t>
+  </si>
+  <si>
+    <t>CD3</t>
+  </si>
+  <si>
+    <t>A0452</t>
+  </si>
+  <si>
+    <t>A0-ABC</t>
+  </si>
+  <si>
+    <t>1:1,000</t>
+  </si>
+  <si>
+    <t>PD-1</t>
+  </si>
+  <si>
+    <t>EH33</t>
+  </si>
+  <si>
+    <t>EH-ABC</t>
+  </si>
+  <si>
+    <t>1:11,000</t>
+  </si>
+  <si>
+    <t>1:150</t>
+  </si>
+  <si>
+    <t>Cytokeratin</t>
+  </si>
+  <si>
+    <t>A1/A3</t>
+  </si>
+  <si>
+    <t>A1-ABC</t>
+  </si>
+  <si>
+    <t>1:2000</t>
+  </si>
+  <si>
+    <t>1:50</t>
+  </si>
+  <si>
     <t>MA036-001</t>
   </si>
   <si>
@@ -317,94 +407,7 @@
     <t>C1D1</t>
   </si>
   <si>
-    <t>CD8</t>
-  </si>
-  <si>
-    <t>C8/144b</t>
-  </si>
-  <si>
-    <t>DAKO</t>
-  </si>
-  <si>
-    <t>C8-ABC</t>
-  </si>
-  <si>
-    <t>DV</t>
-  </si>
-  <si>
-    <t>1:100</t>
-  </si>
-  <si>
-    <t>PD-L1</t>
-  </si>
-  <si>
-    <t>9A11</t>
-  </si>
-  <si>
-    <t>CST</t>
-  </si>
-  <si>
-    <t>9A-ABC</t>
-  </si>
-  <si>
-    <t>1:500</t>
-  </si>
-  <si>
-    <t>VENTANA</t>
-  </si>
-  <si>
-    <t>1:200</t>
-  </si>
-  <si>
-    <t>CD3</t>
-  </si>
-  <si>
-    <t>A0452</t>
-  </si>
-  <si>
-    <t>A0-ABC</t>
-  </si>
-  <si>
-    <t>PD-1</t>
-  </si>
-  <si>
-    <t>EH33</t>
-  </si>
-  <si>
-    <t>EH-ABC</t>
-  </si>
-  <si>
-    <t>1:150</t>
-  </si>
-  <si>
-    <t>Cytokeratin</t>
-  </si>
-  <si>
-    <t>A1/A3</t>
-  </si>
-  <si>
-    <t>A1-ABC</t>
-  </si>
-  <si>
-    <t>1:2000</t>
-  </si>
-  <si>
-    <t>1:50</t>
-  </si>
-  <si>
-    <t>1:5000</t>
-  </si>
-  <si>
-    <t>1:1000</t>
-  </si>
-  <si>
-    <t>1:11000</t>
-  </si>
-  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -513,8 +516,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -532,16 +535,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N215"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -896,21 +896,21 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -942,7 +942,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -964,7 +964,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -986,7 +986,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1008,7 +1008,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1030,7 +1030,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1052,7 +1052,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1074,7 +1074,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1096,7 +1096,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1118,7 +1118,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1140,7 +1140,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1155,21 +1155,21 @@
       <c r="N12" s="1"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1220,16 +1220,16 @@
         <v>16</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F16" s="5">
         <v>3983272</v>
@@ -1241,21 +1241,21 @@
         <v>520</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="L16" s="11">
+        <v>55</v>
+      </c>
+      <c r="L16" s="10">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="10">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="10">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1264,16 +1264,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F17" s="5">
         <v>29387234</v>
@@ -1285,21 +1285,21 @@
         <v>540</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="L17" s="11">
+        <v>62</v>
+      </c>
+      <c r="L17" s="10">
         <v>7.6388888888888886E-3</v>
       </c>
-      <c r="M17" s="11">
+      <c r="M17" s="10">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N17" s="11">
+      <c r="N17" s="10">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1308,16 +1308,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="F18" s="5">
         <v>2881947</v>
@@ -1329,21 +1329,21 @@
         <v>570</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="L18" s="12">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="M18" s="11">
+        <v>62</v>
+      </c>
+      <c r="L18" s="10">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="M18" s="10">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="10">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1352,16 +1352,16 @@
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="F19" s="5">
         <v>293872</v>
@@ -1373,21 +1373,21 @@
         <v>620</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="L19" s="11">
-        <v>7.6388888888888886E-3</v>
-      </c>
-      <c r="M19" s="11">
+        <v>71</v>
+      </c>
+      <c r="L19" s="10">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="M19" s="10">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N19" s="11">
+      <c r="N19" s="10">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1396,16 +1396,16 @@
         <v>16</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F20" s="5">
         <v>392835</v>
@@ -1417,21 +1417,21 @@
         <v>690</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="L20" s="11">
+        <v>76</v>
+      </c>
+      <c r="L20" s="10">
         <v>9.7222222222222224E-3</v>
       </c>
-      <c r="M20" s="11">
+      <c r="M20" s="10">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="10">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -2437,7 +2437,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"proprietary,random forest classifier"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L16:N17 M18:N18 L19:N215" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L16:N215" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
@@ -2451,8 +2451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2484,17 +2484,18 @@
       <c r="N1" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2527,101 +2528,113 @@
       <c r="J4" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="K4" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="10">
-        <v>35796</v>
-      </c>
-      <c r="G5" s="10">
+      <c r="G5" s="12">
         <v>35797</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>52</v>
+      <c r="H5" s="12">
+        <v>35797</v>
+      </c>
+      <c r="I5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="10">
-        <v>35797</v>
-      </c>
-      <c r="G6" s="10">
-        <v>35797</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>52</v>
+      <c r="B6" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="12">
+        <v>35798</v>
+      </c>
+      <c r="H6" s="12">
+        <v>35798</v>
+      </c>
+      <c r="I6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="10">
-        <v>35798</v>
-      </c>
-      <c r="G7" s="10">
-        <v>35797</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="B7" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>52</v>
+      <c r="E7" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="12">
+        <v>35799</v>
+      </c>
+      <c r="H7" s="12">
+        <v>35799</v>
+      </c>
+      <c r="I7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -3611,13 +3624,13 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B3:K3"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="F5:G204" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>AND(ISNUMBER(F5:F204),LEFT(CELL("format",F5:F204),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G5:H204" xr:uid="{00000000-0002-0000-0100-000000000000}">
+      <formula1>AND(ISNUMBER(G5:G204),LEFT(CELL("format",G5:G204),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H204" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I204" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Remove duplicate items (#52)
* Edited micsss_assay and mif_assay and created imaging_data

* Regenerated and validated json templates

* Added properties to artifact.json

* Deleted image.json, edited artifact.json to artifact_core.json

* Edited artifact.json reference

* added missing docs
</commit_message>
<xml_diff>
--- a/template_examples/mIF_template.xlsx
+++ b/template_examples/mIF_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFA8E12-3166-7343-B4C4-AFD35169C723}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478EAFFD-1742-B94D-BB85-373DD1D8B4C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4180" yWindow="-20100" windowWidth="22200" windowHeight="16560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-860" yWindow="-19460" windowWidth="22680" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mIF_template" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="92">
   <si>
     <t>#t</t>
   </si>
@@ -236,6 +236,9 @@
     <t>TIME POINT</t>
   </si>
   <si>
+    <t>PROTOCOL_NAME</t>
+  </si>
+  <si>
     <t>STAINING DATE</t>
   </si>
   <si>
@@ -263,18 +266,105 @@
     <t>auto</t>
   </si>
   <si>
-    <t>Leica Model</t>
+    <t>Leica Bon RX</t>
   </si>
   <si>
     <t>InForm</t>
   </si>
   <si>
+    <t>2.4.2</t>
+  </si>
+  <si>
     <t>proprietary</t>
   </si>
   <si>
     <t>T-Cell HNSC</t>
   </si>
   <si>
+    <t>CD8</t>
+  </si>
+  <si>
+    <t>C8/144b</t>
+  </si>
+  <si>
+    <t>DAKO</t>
+  </si>
+  <si>
+    <t>C8-ABC</t>
+  </si>
+  <si>
+    <t>1:5,000</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>1:100</t>
+  </si>
+  <si>
+    <t>PD-L1</t>
+  </si>
+  <si>
+    <t>9A11</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>9A-ABC</t>
+  </si>
+  <si>
+    <t>1:500</t>
+  </si>
+  <si>
+    <t>VENTANA</t>
+  </si>
+  <si>
+    <t>1:200</t>
+  </si>
+  <si>
+    <t>CD3</t>
+  </si>
+  <si>
+    <t>A0452</t>
+  </si>
+  <si>
+    <t>A0-ABC</t>
+  </si>
+  <si>
+    <t>1:1,000</t>
+  </si>
+  <si>
+    <t>PD-1</t>
+  </si>
+  <si>
+    <t>EH33</t>
+  </si>
+  <si>
+    <t>EH-ABC</t>
+  </si>
+  <si>
+    <t>1:11,000</t>
+  </si>
+  <si>
+    <t>1:150</t>
+  </si>
+  <si>
+    <t>Cytokeratin</t>
+  </si>
+  <si>
+    <t>A1/A3</t>
+  </si>
+  <si>
+    <t>A1-ABC</t>
+  </si>
+  <si>
+    <t>1:2000</t>
+  </si>
+  <si>
+    <t>1:50</t>
+  </si>
+  <si>
     <t>MA036-001</t>
   </si>
   <si>
@@ -317,94 +407,7 @@
     <t>C1D1</t>
   </si>
   <si>
-    <t>CD8</t>
-  </si>
-  <si>
-    <t>C8/144b</t>
-  </si>
-  <si>
-    <t>DAKO</t>
-  </si>
-  <si>
-    <t>C8-ABC</t>
-  </si>
-  <si>
-    <t>DV</t>
-  </si>
-  <si>
-    <t>1:100</t>
-  </si>
-  <si>
-    <t>PD-L1</t>
-  </si>
-  <si>
-    <t>9A11</t>
-  </si>
-  <si>
-    <t>CST</t>
-  </si>
-  <si>
-    <t>9A-ABC</t>
-  </si>
-  <si>
-    <t>1:500</t>
-  </si>
-  <si>
-    <t>VENTANA</t>
-  </si>
-  <si>
-    <t>1:200</t>
-  </si>
-  <si>
-    <t>CD3</t>
-  </si>
-  <si>
-    <t>A0452</t>
-  </si>
-  <si>
-    <t>A0-ABC</t>
-  </si>
-  <si>
-    <t>PD-1</t>
-  </si>
-  <si>
-    <t>EH33</t>
-  </si>
-  <si>
-    <t>EH-ABC</t>
-  </si>
-  <si>
-    <t>1:150</t>
-  </si>
-  <si>
-    <t>Cytokeratin</t>
-  </si>
-  <si>
-    <t>A1/A3</t>
-  </si>
-  <si>
-    <t>A1-ABC</t>
-  </si>
-  <si>
-    <t>1:2000</t>
-  </si>
-  <si>
-    <t>1:50</t>
-  </si>
-  <si>
-    <t>1:5000</t>
-  </si>
-  <si>
-    <t>1:1000</t>
-  </si>
-  <si>
-    <t>1:11000</t>
-  </si>
-  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -513,8 +516,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -532,16 +535,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N215"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -896,21 +896,21 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -942,7 +942,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -964,7 +964,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -986,7 +986,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1008,7 +1008,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1030,7 +1030,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1052,7 +1052,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1074,7 +1074,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1096,7 +1096,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1118,7 +1118,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1140,7 +1140,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1155,21 +1155,21 @@
       <c r="N12" s="1"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1220,16 +1220,16 @@
         <v>16</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F16" s="5">
         <v>3983272</v>
@@ -1241,21 +1241,21 @@
         <v>520</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="L16" s="11">
+        <v>55</v>
+      </c>
+      <c r="L16" s="10">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="10">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="10">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1264,16 +1264,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F17" s="5">
         <v>29387234</v>
@@ -1285,21 +1285,21 @@
         <v>540</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="L17" s="11">
+        <v>62</v>
+      </c>
+      <c r="L17" s="10">
         <v>7.6388888888888886E-3</v>
       </c>
-      <c r="M17" s="11">
+      <c r="M17" s="10">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N17" s="11">
+      <c r="N17" s="10">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1308,16 +1308,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="F18" s="5">
         <v>2881947</v>
@@ -1329,21 +1329,21 @@
         <v>570</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="L18" s="12">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="M18" s="11">
+        <v>62</v>
+      </c>
+      <c r="L18" s="10">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="M18" s="10">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="10">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1352,16 +1352,16 @@
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="F19" s="5">
         <v>293872</v>
@@ -1373,21 +1373,21 @@
         <v>620</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="L19" s="11">
-        <v>7.6388888888888886E-3</v>
-      </c>
-      <c r="M19" s="11">
+        <v>71</v>
+      </c>
+      <c r="L19" s="10">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="M19" s="10">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N19" s="11">
+      <c r="N19" s="10">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1396,16 +1396,16 @@
         <v>16</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F20" s="5">
         <v>392835</v>
@@ -1417,21 +1417,21 @@
         <v>690</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="L20" s="11">
+        <v>76</v>
+      </c>
+      <c r="L20" s="10">
         <v>9.7222222222222224E-3</v>
       </c>
-      <c r="M20" s="11">
+      <c r="M20" s="10">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="10">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -2437,7 +2437,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"proprietary,random forest classifier"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L16:N17 M18:N18 L19:N215" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L16:N215" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
@@ -2451,8 +2451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2484,17 +2484,18 @@
       <c r="N1" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2527,101 +2528,113 @@
       <c r="J4" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="K4" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="10">
-        <v>35796</v>
-      </c>
-      <c r="G5" s="10">
+      <c r="G5" s="12">
         <v>35797</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>52</v>
+      <c r="H5" s="12">
+        <v>35797</v>
+      </c>
+      <c r="I5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="10">
-        <v>35797</v>
-      </c>
-      <c r="G6" s="10">
-        <v>35797</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>52</v>
+      <c r="B6" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="12">
+        <v>35798</v>
+      </c>
+      <c r="H6" s="12">
+        <v>35798</v>
+      </c>
+      <c r="I6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="10">
-        <v>35798</v>
-      </c>
-      <c r="G7" s="10">
-        <v>35797</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="B7" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>52</v>
+      <c r="E7" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="12">
+        <v>35799</v>
+      </c>
+      <c r="H7" s="12">
+        <v>35799</v>
+      </c>
+      <c r="I7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -3611,13 +3624,13 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B3:K3"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="F5:G204" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>AND(ISNUMBER(F5:F204),LEFT(CELL("format",F5:F204),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G5:H204" xr:uid="{00000000-0002-0000-0100-000000000000}">
+      <formula1>AND(ISNUMBER(G5:G204),LEFT(CELL("format",G5:G204),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H204" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I204" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Changed worksheet name for mif_template and micsss_template
</commit_message>
<xml_diff>
--- a/template_examples/mIF_template.xlsx
+++ b/template_examples/mIF_template.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478EAFFD-1742-B94D-BB85-373DD1D8B4C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637039CC-78D4-7941-9504-6C54559B3CC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-860" yWindow="-19460" windowWidth="22680" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23440" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="mIF_template" sheetId="1" r:id="rId1"/>
+    <sheet name="mIF" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="93">
   <si>
     <t>#t</t>
   </si>
@@ -260,13 +260,13 @@
     <t>Multiplex Immunofluorescence</t>
   </si>
   <si>
-    <t>Vectra 2.0</t>
+    <t>Hamamatsu</t>
   </si>
   <si>
     <t>auto</t>
   </si>
   <si>
-    <t>Leica Bon RX</t>
+    <t>Leica Bond RX</t>
   </si>
   <si>
     <t>InForm</t>
@@ -278,103 +278,109 @@
     <t>proprietary</t>
   </si>
   <si>
+    <t>T-Cell HSNC</t>
+  </si>
+  <si>
+    <t>CD8</t>
+  </si>
+  <si>
+    <t>C8/144b</t>
+  </si>
+  <si>
+    <t>DAKO</t>
+  </si>
+  <si>
+    <t>C8-ABC</t>
+  </si>
+  <si>
+    <t>1:5,000</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>1:100</t>
+  </si>
+  <si>
+    <t>PD-L1</t>
+  </si>
+  <si>
+    <t>9A11</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>9A-ABC</t>
+  </si>
+  <si>
+    <t>1:500</t>
+  </si>
+  <si>
+    <t>VENTANA</t>
+  </si>
+  <si>
+    <t>1:200</t>
+  </si>
+  <si>
+    <t>CD3</t>
+  </si>
+  <si>
+    <t>A0452</t>
+  </si>
+  <si>
+    <t>A0-ABC</t>
+  </si>
+  <si>
+    <t>1:1,000</t>
+  </si>
+  <si>
+    <t>PD-1</t>
+  </si>
+  <si>
+    <t>EH33</t>
+  </si>
+  <si>
+    <t>EH-ABC</t>
+  </si>
+  <si>
+    <t>1:11,000</t>
+  </si>
+  <si>
+    <t>1:150</t>
+  </si>
+  <si>
+    <t>Cytokeratin</t>
+  </si>
+  <si>
+    <t>A1/A3</t>
+  </si>
+  <si>
+    <t>A1-ABC</t>
+  </si>
+  <si>
+    <t>1:2000</t>
+  </si>
+  <si>
+    <t>1:50</t>
+  </si>
+  <si>
+    <t>MA036-001</t>
+  </si>
+  <si>
+    <t>MA036-001 PRE</t>
+  </si>
+  <si>
+    <t>07FK 099</t>
+  </si>
+  <si>
+    <t>PRE</t>
+  </si>
+  <si>
     <t>T-Cell HNSC</t>
   </si>
   <si>
-    <t>CD8</t>
-  </si>
-  <si>
-    <t>C8/144b</t>
-  </si>
-  <si>
-    <t>DAKO</t>
-  </si>
-  <si>
-    <t>C8-ABC</t>
-  </si>
-  <si>
-    <t>1:5,000</t>
-  </si>
-  <si>
-    <t>DV</t>
-  </si>
-  <si>
-    <t>1:100</t>
-  </si>
-  <si>
-    <t>PD-L1</t>
-  </si>
-  <si>
-    <t>9A11</t>
-  </si>
-  <si>
-    <t>CST</t>
-  </si>
-  <si>
-    <t>9A-ABC</t>
-  </si>
-  <si>
-    <t>1:500</t>
-  </si>
-  <si>
-    <t>VENTANA</t>
-  </si>
-  <si>
-    <t>1:200</t>
-  </si>
-  <si>
-    <t>CD3</t>
-  </si>
-  <si>
-    <t>A0452</t>
-  </si>
-  <si>
-    <t>A0-ABC</t>
-  </si>
-  <si>
-    <t>1:1,000</t>
-  </si>
-  <si>
-    <t>PD-1</t>
-  </si>
-  <si>
-    <t>EH33</t>
-  </si>
-  <si>
-    <t>EH-ABC</t>
-  </si>
-  <si>
-    <t>1:11,000</t>
-  </si>
-  <si>
-    <t>1:150</t>
-  </si>
-  <si>
-    <t>Cytokeratin</t>
-  </si>
-  <si>
-    <t>A1/A3</t>
-  </si>
-  <si>
-    <t>A1-ABC</t>
-  </si>
-  <si>
-    <t>1:2000</t>
-  </si>
-  <si>
-    <t>1:50</t>
-  </si>
-  <si>
-    <t>MA036-001</t>
-  </si>
-  <si>
-    <t>MA036-001 PRE</t>
-  </si>
-  <si>
-    <t>07FK 099</t>
-  </si>
-  <si>
-    <t>PRE</t>
+    <t>Yes</t>
   </si>
   <si>
     <t>ABC_INFORM</t>
@@ -405,9 +411,6 @@
   </si>
   <si>
     <t>C1D1</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -526,6 +529,9 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -534,9 +540,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -882,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1249,13 +1252,13 @@
       <c r="K16" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="7">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="7">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N16" s="10">
+      <c r="N16" s="7">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1263,7 +1266,7 @@
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>56</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1293,13 +1296,13 @@
       <c r="K17" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="7">
         <v>7.6388888888888886E-3</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="7">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N17" s="10">
+      <c r="N17" s="7">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1307,7 +1310,7 @@
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>63</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -1337,13 +1340,13 @@
       <c r="K18" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="7">
         <v>8.3333333333333332E-3</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="7">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N18" s="10">
+      <c r="N18" s="7">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1381,13 +1384,13 @@
       <c r="K19" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="7">
         <v>9.0277777777777787E-3</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="7">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N19" s="10">
+      <c r="N19" s="7">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1395,7 +1398,7 @@
       <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>72</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1425,13 +1428,13 @@
       <c r="K20" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="7">
         <v>9.7222222222222224E-3</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="7">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N20" s="10">
+      <c r="N20" s="7">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -2452,7 +2455,7 @@
   <dimension ref="A1:N204"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2549,7 +2552,7 @@
         <v>80</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="G5" s="12">
         <v>35797</v>
@@ -2558,13 +2561,13 @@
         <v>35797</v>
       </c>
       <c r="I5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -2572,19 +2575,19 @@
         <v>16</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="G6" s="12">
         <v>35798</v>
@@ -2593,13 +2596,13 @@
         <v>35798</v>
       </c>
       <c r="I6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -2607,19 +2610,19 @@
         <v>16</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="G7" s="12">
         <v>35799</v>
@@ -2628,13 +2631,13 @@
         <v>35799</v>
       </c>
       <c r="I7" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Changed worksheet name for mif_template and micsss_template (#82)
</commit_message>
<xml_diff>
--- a/template_examples/mIF_template.xlsx
+++ b/template_examples/mIF_template.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478EAFFD-1742-B94D-BB85-373DD1D8B4C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637039CC-78D4-7941-9504-6C54559B3CC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-860" yWindow="-19460" windowWidth="22680" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23440" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="mIF_template" sheetId="1" r:id="rId1"/>
+    <sheet name="mIF" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="93">
   <si>
     <t>#t</t>
   </si>
@@ -260,13 +260,13 @@
     <t>Multiplex Immunofluorescence</t>
   </si>
   <si>
-    <t>Vectra 2.0</t>
+    <t>Hamamatsu</t>
   </si>
   <si>
     <t>auto</t>
   </si>
   <si>
-    <t>Leica Bon RX</t>
+    <t>Leica Bond RX</t>
   </si>
   <si>
     <t>InForm</t>
@@ -278,103 +278,109 @@
     <t>proprietary</t>
   </si>
   <si>
+    <t>T-Cell HSNC</t>
+  </si>
+  <si>
+    <t>CD8</t>
+  </si>
+  <si>
+    <t>C8/144b</t>
+  </si>
+  <si>
+    <t>DAKO</t>
+  </si>
+  <si>
+    <t>C8-ABC</t>
+  </si>
+  <si>
+    <t>1:5,000</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>1:100</t>
+  </si>
+  <si>
+    <t>PD-L1</t>
+  </si>
+  <si>
+    <t>9A11</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>9A-ABC</t>
+  </si>
+  <si>
+    <t>1:500</t>
+  </si>
+  <si>
+    <t>VENTANA</t>
+  </si>
+  <si>
+    <t>1:200</t>
+  </si>
+  <si>
+    <t>CD3</t>
+  </si>
+  <si>
+    <t>A0452</t>
+  </si>
+  <si>
+    <t>A0-ABC</t>
+  </si>
+  <si>
+    <t>1:1,000</t>
+  </si>
+  <si>
+    <t>PD-1</t>
+  </si>
+  <si>
+    <t>EH33</t>
+  </si>
+  <si>
+    <t>EH-ABC</t>
+  </si>
+  <si>
+    <t>1:11,000</t>
+  </si>
+  <si>
+    <t>1:150</t>
+  </si>
+  <si>
+    <t>Cytokeratin</t>
+  </si>
+  <si>
+    <t>A1/A3</t>
+  </si>
+  <si>
+    <t>A1-ABC</t>
+  </si>
+  <si>
+    <t>1:2000</t>
+  </si>
+  <si>
+    <t>1:50</t>
+  </si>
+  <si>
+    <t>MA036-001</t>
+  </si>
+  <si>
+    <t>MA036-001 PRE</t>
+  </si>
+  <si>
+    <t>07FK 099</t>
+  </si>
+  <si>
+    <t>PRE</t>
+  </si>
+  <si>
     <t>T-Cell HNSC</t>
   </si>
   <si>
-    <t>CD8</t>
-  </si>
-  <si>
-    <t>C8/144b</t>
-  </si>
-  <si>
-    <t>DAKO</t>
-  </si>
-  <si>
-    <t>C8-ABC</t>
-  </si>
-  <si>
-    <t>1:5,000</t>
-  </si>
-  <si>
-    <t>DV</t>
-  </si>
-  <si>
-    <t>1:100</t>
-  </si>
-  <si>
-    <t>PD-L1</t>
-  </si>
-  <si>
-    <t>9A11</t>
-  </si>
-  <si>
-    <t>CST</t>
-  </si>
-  <si>
-    <t>9A-ABC</t>
-  </si>
-  <si>
-    <t>1:500</t>
-  </si>
-  <si>
-    <t>VENTANA</t>
-  </si>
-  <si>
-    <t>1:200</t>
-  </si>
-  <si>
-    <t>CD3</t>
-  </si>
-  <si>
-    <t>A0452</t>
-  </si>
-  <si>
-    <t>A0-ABC</t>
-  </si>
-  <si>
-    <t>1:1,000</t>
-  </si>
-  <si>
-    <t>PD-1</t>
-  </si>
-  <si>
-    <t>EH33</t>
-  </si>
-  <si>
-    <t>EH-ABC</t>
-  </si>
-  <si>
-    <t>1:11,000</t>
-  </si>
-  <si>
-    <t>1:150</t>
-  </si>
-  <si>
-    <t>Cytokeratin</t>
-  </si>
-  <si>
-    <t>A1/A3</t>
-  </si>
-  <si>
-    <t>A1-ABC</t>
-  </si>
-  <si>
-    <t>1:2000</t>
-  </si>
-  <si>
-    <t>1:50</t>
-  </si>
-  <si>
-    <t>MA036-001</t>
-  </si>
-  <si>
-    <t>MA036-001 PRE</t>
-  </si>
-  <si>
-    <t>07FK 099</t>
-  </si>
-  <si>
-    <t>PRE</t>
+    <t>Yes</t>
   </si>
   <si>
     <t>ABC_INFORM</t>
@@ -405,9 +411,6 @@
   </si>
   <si>
     <t>C1D1</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -526,6 +529,9 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -534,9 +540,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -882,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1249,13 +1252,13 @@
       <c r="K16" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="7">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="7">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N16" s="10">
+      <c r="N16" s="7">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1263,7 +1266,7 @@
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>56</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1293,13 +1296,13 @@
       <c r="K17" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="7">
         <v>7.6388888888888886E-3</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="7">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N17" s="10">
+      <c r="N17" s="7">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1307,7 +1310,7 @@
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>63</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -1337,13 +1340,13 @@
       <c r="K18" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="7">
         <v>8.3333333333333332E-3</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="7">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N18" s="10">
+      <c r="N18" s="7">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1381,13 +1384,13 @@
       <c r="K19" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="7">
         <v>9.0277777777777787E-3</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="7">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N19" s="10">
+      <c r="N19" s="7">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -1395,7 +1398,7 @@
       <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>72</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1425,13 +1428,13 @@
       <c r="K20" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="7">
         <v>9.7222222222222224E-3</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="7">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="N20" s="10">
+      <c r="N20" s="7">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
@@ -2452,7 +2455,7 @@
   <dimension ref="A1:N204"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2549,7 +2552,7 @@
         <v>80</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="G5" s="12">
         <v>35797</v>
@@ -2558,13 +2561,13 @@
         <v>35797</v>
       </c>
       <c r="I5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -2572,19 +2575,19 @@
         <v>16</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="G6" s="12">
         <v>35798</v>
@@ -2593,13 +2596,13 @@
         <v>35798</v>
       </c>
       <c r="I6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -2607,19 +2610,19 @@
         <v>16</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="G7" s="12">
         <v>35799</v>
@@ -2628,13 +2631,13 @@
         <v>35799</v>
       </c>
       <c r="I7" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>